<commit_message>
added sony camera tidied code
</commit_message>
<xml_diff>
--- a/lensformulae/cameras.xlsx
+++ b/lensformulae/cameras.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob\Documents\R\dev\photography\lensformulae\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC00CE4F-6C13-4B09-A613-51E4EF84A647}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7737045C-67E9-43A4-8B2C-019C037719E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{57797F44-4CEF-4E41-BABA-46EBDF0AF24A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>image size</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>MPinch</t>
+  </si>
+  <si>
+    <t>Sony a7ii</t>
   </si>
 </sst>
 </file>
@@ -994,10 +997,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61CFF128-252E-4A54-A9B9-13C60103D7E6}">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L6"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1111,7 +1114,7 @@
         <v>4025</v>
       </c>
       <c r="F3" s="1">
-        <f t="shared" ref="F3:F6" si="0">B3/D3*1000</f>
+        <f t="shared" ref="F3:F7" si="0">B3/D3*1000</f>
         <v>5.945677376614773</v>
       </c>
       <c r="G3" s="1">
@@ -1278,6 +1281,51 @@
       <c r="L6" s="4" t="str">
         <f t="shared" si="5"/>
         <v>- 70x87 inch</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>35.799999999999997</v>
+      </c>
+      <c r="C7">
+        <v>23.9</v>
+      </c>
+      <c r="D7">
+        <v>6000</v>
+      </c>
+      <c r="E7">
+        <v>4000</v>
+      </c>
+      <c r="F7" s="1">
+        <f t="shared" si="0"/>
+        <v>5.9666666666666659</v>
+      </c>
+      <c r="G7" s="1">
+        <f t="shared" ref="G7" si="7">C7/E7*1000</f>
+        <v>5.9749999999999996</v>
+      </c>
+      <c r="H7" s="1">
+        <f t="shared" ref="H7" si="8">AVERAGE(F7:G7)</f>
+        <v>5.9708333333333332</v>
+      </c>
+      <c r="I7" s="3">
+        <f>I6</f>
+        <v>174.625</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ref="J7" si="9">I7/H7</f>
+        <v>29.246336357292392</v>
+      </c>
+      <c r="K7" s="4" t="str">
+        <f t="shared" ref="K7" si="10">_xlfn.CONCAT("- ",ROUND(B7*J7,0),"x",ROUND(C7*J7,0)," mm")</f>
+        <v>- 1047x699 mm</v>
+      </c>
+      <c r="L7" s="4" t="str">
+        <f t="shared" ref="L7" si="11">_xlfn.CONCAT("- ",ROUND(B7*J7/25.4,0),"x",ROUND(C7*J7/25.4,0)," inch")</f>
+        <v>- 41x28 inch</v>
       </c>
     </row>
   </sheetData>

</xml_diff>